<commit_message>
Added cluster information on couples excel page
</commit_message>
<xml_diff>
--- a/example_output/pySODA_results_example_image.xlsx
+++ b/example_output/pySODA_results_example_image.xlsx
@@ -37,7 +37,7 @@
     <t>Weighted mean coupling distance</t>
   </si>
   <si>
-    <t>0_M-PSD_GAMA594-R-Bassoon-GARSTAR635_15nm_naive(noTTX)_block_02.msr_2_STED_merged.tif</t>
+    <t>R-Homer_GARSTAR635_M-Bassoon_GAMAlexa594_0MgGlyBic_02.tif</t>
   </si>
 </sst>
 </file>
@@ -403,22 +403,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1435</v>
+        <v>1900</v>
       </c>
       <c r="C2">
-        <v>1625</v>
+        <v>994</v>
       </c>
       <c r="D2">
-        <v>641</v>
+        <v>321</v>
       </c>
       <c r="E2">
-        <v>0.2141207395202776</v>
+        <v>0.05130075048611943</v>
       </c>
       <c r="F2">
-        <v>0.189085083822522</v>
+        <v>0.0980597846314154</v>
       </c>
       <c r="G2">
-        <v>6.429981801837614</v>
+        <v>8.131633999137502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>